<commit_message>
Working trends for baseline scen
</commit_message>
<xml_diff>
--- a/inputs/demo_demo_input.xlsx
+++ b/inputs/demo_demo_input.xlsx
@@ -3398,7 +3398,7 @@
         <xdr:cNvPr id="2049" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000001080000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000001080000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3455,7 +3455,7 @@
         <xdr:cNvPr id="2" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3512,7 +3512,7 @@
         <xdr:cNvPr id="3" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000003000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3569,7 +3569,7 @@
         <xdr:cNvPr id="4" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000004000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3626,7 +3626,7 @@
         <xdr:cNvPr id="5" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000005000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3683,7 +3683,7 @@
         <xdr:cNvPr id="6" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000006000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000006000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3740,7 +3740,7 @@
         <xdr:cNvPr id="7" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000007000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000007000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3797,7 +3797,7 @@
         <xdr:cNvPr id="8" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000008000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000008000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3854,7 +3854,7 @@
         <xdr:cNvPr id="9" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000009000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000009000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3911,7 +3911,7 @@
         <xdr:cNvPr id="10" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-00000A000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00000A000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3968,7 +3968,7 @@
         <xdr:cNvPr id="11" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-00000B000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00000B000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4025,7 +4025,7 @@
         <xdr:cNvPr id="12" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-00000C000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00000C000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4082,7 +4082,7 @@
         <xdr:cNvPr id="13" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-00000D000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00000D000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4139,7 +4139,7 @@
         <xdr:cNvPr id="14" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-00000E000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00000E000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4196,7 +4196,7 @@
         <xdr:cNvPr id="15" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-00000F000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00000F000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4253,7 +4253,7 @@
         <xdr:cNvPr id="16" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000010000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000010000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4310,7 +4310,7 @@
         <xdr:cNvPr id="17" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000011000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000011000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4367,7 +4367,7 @@
         <xdr:cNvPr id="18" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000012000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000012000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4416,7 +4416,7 @@
         <xdr:cNvPr id="19" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000013000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000013000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4785,7 +4785,7 @@
   </sheetPr>
   <dimension ref="A1:E63"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
@@ -11564,12 +11564,6 @@
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="BiU9BXNF+INgNxSFtHuqKvDgOHy4i8LHe4WBopPE5oAPe1uu8rzbQfKL4uxCQ4dbx+6qcxc95feCcYk3II7eJw==" saltValue="oFkUqZTkt+d2Svo646TgPw==" spinCount="100000" sheet="1" scenarios="1" selectLockedCells="1"/>
   <mergeCells count="15">
-    <mergeCell ref="B19:B21"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="B5:B7"/>
-    <mergeCell ref="B8:B10"/>
-    <mergeCell ref="B11:B13"/>
-    <mergeCell ref="B14:B16"/>
     <mergeCell ref="B42:B44"/>
     <mergeCell ref="B45:B47"/>
     <mergeCell ref="B48:B50"/>
@@ -11579,6 +11573,12 @@
     <mergeCell ref="B31:B33"/>
     <mergeCell ref="B36:B38"/>
     <mergeCell ref="B39:B41"/>
+    <mergeCell ref="B19:B21"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="B14:B16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -18780,7 +18780,7 @@
   </sheetPr>
   <dimension ref="A1:H35"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
@@ -19647,7 +19647,7 @@
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -19783,7 +19783,7 @@
   <dimension ref="A1:P14"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -19869,7 +19869,7 @@
       <c r="N2" s="28"/>
       <c r="O2" s="28"/>
       <c r="P2" s="28">
-        <v>0</v>
+        <v>0.33</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
@@ -19917,14 +19917,12 @@
         <v>143</v>
       </c>
       <c r="C6" s="28">
-        <f>'Nutritional status distribution'!C15*(1/60)+'Nutritional status distribution'!D15*(5/10)+'Nutritional status distribution'!E15*(6/60)+'Nutritional status distribution'!F15*(12/60)+'Nutritional status distribution'!G15*(24/60)</f>
-        <v>0.19703599999999999</v>
+        <f>'Nutritional status distribution'!C15*(1/60)+'Nutritional status distribution'!D15*(5/60)+'Nutritional status distribution'!E15*(6/60)+'Nutritional status distribution'!F15*(12/60)+'Nutritional status distribution'!G15*(36/60)</f>
+        <v>0.22016400000000003</v>
       </c>
       <c r="D6" s="28"/>
       <c r="E6" s="28"/>
-      <c r="F6" s="28">
-        <v>0</v>
-      </c>
+      <c r="F6" s="28"/>
       <c r="G6" s="28"/>
       <c r="H6" s="28"/>
       <c r="I6" s="28"/>
@@ -19935,7 +19933,7 @@
       <c r="N6" s="28"/>
       <c r="O6" s="28"/>
       <c r="P6" s="28">
-        <v>0.18</v>
+        <v>0.19800000000000001</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
@@ -19943,7 +19941,7 @@
         <v>32</v>
       </c>
       <c r="C7" s="28">
-        <f>C8</f>
+        <f>('Nutritional status distribution'!H15*('Demographic projections'!C2/SUM('Demographic projections'!C2:F2))+'Nutritional status distribution'!I15*('Demographic projections'!D2/SUM('Demographic projections'!C2:F2))+'Nutritional status distribution'!J15*('Demographic projections'!E2/SUM('Demographic projections'!C2:F2))+'Nutritional status distribution'!K15*('Demographic projections'!F2/SUM('Demographic projections'!C2:F2)))</f>
         <v>0.18837666072928053</v>
       </c>
       <c r="D7" s="28"/>
@@ -19967,7 +19965,7 @@
         <v>144</v>
       </c>
       <c r="C8" s="28">
-        <f>('Nutritional status distribution'!H15*('Demographic projections'!C2/SUM('Demographic projections'!C2:F2))+'Nutritional status distribution'!I15*('Demographic projections'!D2/SUM('Demographic projections'!C2:F2))+'Nutritional status distribution'!J15*('Demographic projections'!E2/SUM('Demographic projections'!C2:F2))+'Nutritional status distribution'!K15*('Demographic projections'!F2/SUM('Demographic projections'!C2:F2)))</f>
+        <f>('Nutritional status distribution'!L15*('Demographic projections'!C2/SUM('Demographic projections'!C2:F2))+'Nutritional status distribution'!M15*('Demographic projections'!D2/SUM('Demographic projections'!C2:F2))+'Nutritional status distribution'!N15*('Demographic projections'!E2/SUM('Demographic projections'!C2:F2))+'Nutritional status distribution'!O15*('Demographic projections'!F2/SUM('Demographic projections'!C2:F2)))</f>
         <v>0.18837666072928053</v>
       </c>
       <c r="D8" s="28"/>
@@ -19985,7 +19983,7 @@
       <c r="N8" s="28"/>
       <c r="O8" s="28"/>
       <c r="P8" s="28">
-        <v>0.2</v>
+        <v>0.17399999999999999</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
@@ -20020,8 +20018,8 @@
         <v>146</v>
       </c>
       <c r="C11" s="28">
-        <f>(('Breastfeeding distribution'!E2+'Breastfeeding distribution'!E3+'Breastfeeding distribution'!E4)*(6/18)+('Breastfeeding distribution'!F2+'Breastfeeding distribution'!F3+'Breastfeeding distribution'!F4)*(12/18))</f>
-        <v>0.80834605377276669</v>
+        <f>(('Breastfeeding distribution'!E4)*(6/18)+('Breastfeeding distribution'!F4)*(12/18))</f>
+        <v>0.79221422376409367</v>
       </c>
       <c r="D11" s="28"/>
       <c r="E11" s="28"/>
@@ -20047,8 +20045,8 @@
         <v>148</v>
       </c>
       <c r="C13" s="28">
-        <f>(2.5*(1/60)+4.3*(11/60)+6.7*(48/60))/100</f>
-        <v>6.1900000000000004E-2</v>
+        <f>U5_mortality/1000</f>
+        <v>6.7000000000000004E-2</v>
       </c>
       <c r="D13" s="28"/>
       <c r="E13" s="28"/>
@@ -20057,15 +20055,13 @@
       <c r="H13" s="28"/>
       <c r="I13" s="28"/>
       <c r="J13" s="28"/>
-      <c r="K13" s="28">
-        <v>5.8000000000000003E-2</v>
-      </c>
+      <c r="K13" s="28"/>
       <c r="L13" s="28"/>
       <c r="M13" s="28"/>
       <c r="N13" s="28"/>
       <c r="O13" s="28"/>
       <c r="P13" s="28">
-        <v>5.5E-2</v>
+        <v>6.7000000000000004E-2</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
@@ -20073,8 +20069,8 @@
         <v>170</v>
       </c>
       <c r="C14" s="28">
-        <f>maternal_mortality/100</f>
-        <v>4.0099999999999997E-2</v>
+        <f>maternal_mortality/1000</f>
+        <v>4.0099999999999997E-3</v>
       </c>
       <c r="D14" s="28"/>
       <c r="E14" s="28"/>
@@ -20089,7 +20085,7 @@
       <c r="N14" s="28"/>
       <c r="O14" s="28"/>
       <c r="P14" s="28">
-        <v>3.5999999999999997E-2</v>
+        <v>4.0000000000000001E-3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Code has been neatened and streamlined a bit
</commit_message>
<xml_diff>
--- a/inputs/demo_demo_input.xlsx
+++ b/inputs/demo_demo_input.xlsx
@@ -14569,7 +14569,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="56" spans="1:16" s="36" customFormat="1" ht="26" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:16" s="36" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A56" s="121" t="s">
         <v>70</v>
       </c>
@@ -19783,7 +19783,7 @@
   <dimension ref="A1:P14"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -19859,9 +19859,7 @@
       <c r="F2" s="28"/>
       <c r="G2" s="28"/>
       <c r="H2" s="28"/>
-      <c r="I2" s="28">
-        <v>0</v>
-      </c>
+      <c r="I2" s="28"/>
       <c r="J2" s="28"/>
       <c r="K2" s="28"/>
       <c r="L2" s="28"/>
@@ -19898,9 +19896,7 @@
       </c>
       <c r="L4" s="28"/>
       <c r="M4" s="28"/>
-      <c r="N4" s="28">
-        <v>0.05</v>
-      </c>
+      <c r="N4" s="28"/>
       <c r="O4" s="28"/>
       <c r="P4" s="28">
         <v>3.9E-2</v>

</xml_diff>

<commit_message>
Updated efficacy values in demo_demo_input.xlsx and template.xlsx
</commit_message>
<xml_diff>
--- a/inputs/demo_demo_input.xlsx
+++ b/inputs/demo_demo_input.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22430"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dominic.delport\Documents\GitHub\Nutrition\inputs\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{3A74EB16-E57F-43FD-989D-00DC64EFA992}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="-21130" windowWidth="20740" windowHeight="11760" tabRatio="961" activeTab="5"/>
+    <workbookView xWindow="-80" yWindow="-80" windowWidth="19360" windowHeight="10360" tabRatio="885" firstSheet="6" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Baseline year population inputs" sheetId="1" r:id="rId1"/>
@@ -16,10 +22,10 @@
     <sheet name="IYCF packages" sheetId="55" r:id="rId7"/>
     <sheet name="Treatment of SAM" sheetId="60" r:id="rId8"/>
     <sheet name="Programs cost and coverage" sheetId="56" r:id="rId9"/>
-    <sheet name="Program dependencies" sheetId="58" r:id="rId10"/>
-    <sheet name="Reference programs" sheetId="59" state="hidden" r:id="rId11"/>
-    <sheet name="Incidence of conditions" sheetId="7" state="hidden" r:id="rId12"/>
-    <sheet name="Programs target population" sheetId="21" r:id="rId13"/>
+    <sheet name="Reference programs" sheetId="59" state="hidden" r:id="rId10"/>
+    <sheet name="Incidence of conditions" sheetId="7" state="hidden" r:id="rId11"/>
+    <sheet name="Programs target population" sheetId="21" r:id="rId12"/>
+    <sheet name="Program dependencies" sheetId="58" r:id="rId13"/>
     <sheet name="Cost curve options" sheetId="61" state="hidden" r:id="rId14"/>
     <sheet name="Programs family planning" sheetId="54" state="hidden" r:id="rId15"/>
     <sheet name="Programs impacted population" sheetId="62" state="hidden" r:id="rId16"/>
@@ -85,8 +91,16 @@
     <definedName name="term_SGA">'Baseline year population inputs'!$C$47</definedName>
     <definedName name="U5_mortality">'Baseline year population inputs'!$C$39</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -95,12 +109,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Nick Scott</author>
   </authors>
   <commentList>
-    <comment ref="D28" authorId="0">
+    <comment ref="D28" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0800-000001000000}">
       <text>
         <r>
           <rPr>
@@ -163,7 +177,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D30" authorId="0">
+    <comment ref="D30" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0800-000002000000}">
       <text>
         <r>
           <rPr>
@@ -226,7 +240,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D37" authorId="0">
+    <comment ref="D37" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0800-000003000000}">
       <text>
         <r>
           <rPr>
@@ -257,12 +271,12 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Sam</author>
   </authors>
   <commentList>
-    <comment ref="B1" authorId="0">
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0900-000001000000}">
       <text>
         <r>
           <rPr>
@@ -286,7 +300,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C1" authorId="0">
+    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0900-000002000000}">
       <text>
         <r>
           <rPr>
@@ -315,12 +329,12 @@
 </file>
 
 <file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Sam</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0">
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0E00-000001000000}">
       <text>
         <r>
           <rPr>
@@ -358,12 +372,12 @@
 </file>
 
 <file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Nick Scott</author>
   </authors>
   <commentList>
-    <comment ref="A36" authorId="0">
+    <comment ref="A36" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-1200-000001000000}">
       <text>
         <r>
           <rPr>
@@ -392,12 +406,12 @@
 </file>
 
 <file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Nick Scott</author>
   </authors>
   <commentList>
-    <comment ref="B6" authorId="0">
+    <comment ref="B6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-1500-000001000000}">
       <text>
         <r>
           <rPr>
@@ -421,7 +435,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B7" authorId="0">
+    <comment ref="B7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-1500-000002000000}">
       <text>
         <r>
           <rPr>
@@ -1266,12 +1280,12 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="4">
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="0.000"/>
-    <numFmt numFmtId="166" formatCode="0.0%"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="166" formatCode="0.000"/>
+    <numFmt numFmtId="167" formatCode="0.0%"/>
   </numFmts>
   <fonts count="27" x14ac:knownFonts="1">
     <font>
@@ -1579,7 +1593,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2297,7 +2311,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="138">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -2333,8 +2347,8 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -2344,7 +2358,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="3" borderId="1" xfId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="9" fillId="3" borderId="1" xfId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
@@ -2354,16 +2368,16 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="9" fillId="3" borderId="1" xfId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="9" fillId="3" borderId="1" xfId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
@@ -2396,7 +2410,7 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="725" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="725" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="725" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="166" fontId="4" fillId="2" borderId="1" xfId="725" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="4" fillId="2" borderId="1" xfId="725" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="725" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -2411,7 +2425,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="725" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="726" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="726" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="166" fontId="19" fillId="3" borderId="4" xfId="725" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="167" fontId="19" fillId="3" borderId="4" xfId="725" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="725" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -2441,7 +2455,7 @@
     <xf numFmtId="9" fontId="9" fillId="3" borderId="1" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="167" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
       <protection locked="0"/>
     </xf>
@@ -2460,28 +2474,28 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="165" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="10" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="166" fontId="9" fillId="3" borderId="1" xfId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="167" fontId="9" fillId="3" borderId="1" xfId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="167" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="167" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="2" borderId="1" xfId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="167" fontId="4" fillId="2" borderId="1" xfId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="2" borderId="1" xfId="725" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="167" fontId="4" fillId="2" borderId="1" xfId="725" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
       <protection locked="0"/>
     </xf>
@@ -2584,7 +2598,7 @@
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="725" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="725" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="725" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="725" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="725" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="1" fontId="26" fillId="0" borderId="0" xfId="726" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="1" fontId="9" fillId="0" borderId="0" xfId="726" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -2614,7 +2628,7 @@
   </cellXfs>
   <cellStyles count="728">
     <cellStyle name="Comma" xfId="9" builtinId="3"/>
-    <cellStyle name="Comma 2" xfId="727"/>
+    <cellStyle name="Comma 2" xfId="727" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -3338,8 +3352,8 @@
     <cellStyle name="Hyperlink" xfId="721" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="723" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="725"/>
-    <cellStyle name="Normal 3" xfId="726"/>
+    <cellStyle name="Normal 2" xfId="725" xr:uid="{00000000-0005-0000-0000-0000D5020000}"/>
+    <cellStyle name="Normal 3" xfId="726" xr:uid="{00000000-0005-0000-0000-0000D6020000}"/>
     <cellStyle name="Percent" xfId="10" builtinId="5"/>
   </cellStyles>
   <dxfs count="1">
@@ -3398,7 +3412,7 @@
         <xdr:cNvPr id="2049" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000001080000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000001080000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3455,7 +3469,7 @@
         <xdr:cNvPr id="2" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3512,7 +3526,7 @@
         <xdr:cNvPr id="3" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3569,7 +3583,7 @@
         <xdr:cNvPr id="4" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3626,7 +3640,7 @@
         <xdr:cNvPr id="5" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000005000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3683,7 +3697,7 @@
         <xdr:cNvPr id="6" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000006000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000006000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3740,7 +3754,7 @@
         <xdr:cNvPr id="7" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000007000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000007000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3797,7 +3811,7 @@
         <xdr:cNvPr id="8" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000008000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000008000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3854,7 +3868,7 @@
         <xdr:cNvPr id="9" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000009000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000009000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3911,7 +3925,7 @@
         <xdr:cNvPr id="10" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00000A000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00000A000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3968,7 +3982,7 @@
         <xdr:cNvPr id="11" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00000B000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00000B000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4025,7 +4039,7 @@
         <xdr:cNvPr id="12" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00000C000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00000C000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4082,7 +4096,7 @@
         <xdr:cNvPr id="13" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00000D000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00000D000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4139,7 +4153,7 @@
         <xdr:cNvPr id="14" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00000E000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00000E000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4196,7 +4210,7 @@
         <xdr:cNvPr id="15" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00000F000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00000F000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4253,7 +4267,7 @@
         <xdr:cNvPr id="16" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000010000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000010000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4310,7 +4324,7 @@
         <xdr:cNvPr id="17" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000011000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000011000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4367,7 +4381,7 @@
         <xdr:cNvPr id="18" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000012000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000012000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4416,7 +4430,7 @@
         <xdr:cNvPr id="19" name="Rectangle 1" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000013000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000013000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4779,7 +4793,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor rgb="FF007600"/>
   </sheetPr>
@@ -5236,156 +5250,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <tabColor theme="7" tint="-0.249977111117893"/>
-  </sheetPr>
-  <dimension ref="A1:C20"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="53" style="52" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="47.90625" style="35" customWidth="1"/>
-    <col min="3" max="3" width="42.453125" style="35" customWidth="1"/>
-    <col min="4" max="16384" width="11.453125" style="35"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" ht="13" x14ac:dyDescent="0.3">
-      <c r="A1" s="40" t="s">
-        <v>69</v>
-      </c>
-      <c r="B1" s="40" t="s">
-        <v>180</v>
-      </c>
-      <c r="C1" s="40" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="83" t="s">
-        <v>187</v>
-      </c>
-      <c r="B2" s="80" t="s">
-        <v>59</v>
-      </c>
-      <c r="C2" s="80"/>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="83" t="s">
-        <v>208</v>
-      </c>
-      <c r="B3" s="80" t="s">
-        <v>59</v>
-      </c>
-      <c r="C3" s="80"/>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="84" t="s">
-        <v>58</v>
-      </c>
-      <c r="B4" s="80" t="s">
-        <v>136</v>
-      </c>
-      <c r="C4" s="80"/>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="84" t="s">
-        <v>137</v>
-      </c>
-      <c r="B5" s="80" t="s">
-        <v>136</v>
-      </c>
-      <c r="C5" s="80"/>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="84"/>
-      <c r="B6" s="85"/>
-      <c r="C6" s="85"/>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="84"/>
-      <c r="B7" s="85"/>
-      <c r="C7" s="85"/>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="84"/>
-      <c r="B8" s="85"/>
-      <c r="C8" s="85"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="84"/>
-      <c r="B9" s="85"/>
-      <c r="C9" s="85"/>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="84"/>
-      <c r="B10" s="85"/>
-      <c r="C10" s="85"/>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="86"/>
-      <c r="B11" s="85"/>
-      <c r="C11" s="85"/>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="86"/>
-      <c r="B12" s="85"/>
-      <c r="C12" s="85"/>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="86"/>
-      <c r="B13" s="85"/>
-      <c r="C13" s="85"/>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="86"/>
-      <c r="B14" s="85"/>
-      <c r="C14" s="85"/>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="86"/>
-      <c r="B15" s="85"/>
-      <c r="C15" s="85"/>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="86"/>
-      <c r="B16" s="85"/>
-      <c r="C16" s="85"/>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="86"/>
-      <c r="B17" s="85"/>
-      <c r="C17" s="85"/>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="86"/>
-      <c r="B18" s="85"/>
-      <c r="C18" s="85"/>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="84"/>
-      <c r="B19" s="85"/>
-      <c r="C19" s="85"/>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="84"/>
-      <c r="B20" s="85"/>
-      <c r="C20" s="85"/>
-    </row>
-  </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="mJIhFbJiXwMDYdaTQpBnnIuyYOuT68NH0zRKA9hB05n6uZvdwWxrgEXuFwGJ+96DUDA/ASxdRlcLT7WZRHSmMg==" saltValue="bb4cIfhca5ee56tuIEArcQ==" spinCount="100000" sheet="1" scenarios="1" selectLockedCells="1"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
-  <legacyDrawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <sheetPr>
     <tabColor theme="0" tint="-0.249977111117893"/>
   </sheetPr>
@@ -5482,8 +5347,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <sheetPr>
     <tabColor theme="0" tint="-0.34998626667073579"/>
   </sheetPr>
@@ -5596,8 +5461,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <sheetPr>
     <tabColor theme="0" tint="-0.249977111117893"/>
   </sheetPr>
@@ -7307,7 +7172,7 @@
     </row>
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="8AA2I9UZPCvjoGOxL0MMyqqXoHDNS7n4JtfrsQRho74JNJJKUigxuy0/aEjLs4m9INQV0OZqejhY0qqpkSRx4A==" saltValue="BKXFXqwFrNK8M/n7gCZbMQ==" spinCount="100000" sheet="1" scenarios="1" selectLockedCells="1"/>
-  <sortState ref="B14:O21">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B14:O21">
     <sortCondition ref="B14:B21"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -7315,8 +7180,157 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+  <sheetPr>
+    <tabColor theme="7" tint="-0.249977111117893"/>
+  </sheetPr>
+  <dimension ref="A1:C20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="53" style="52" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="47.90625" style="35" customWidth="1"/>
+    <col min="3" max="3" width="42.453125" style="35" customWidth="1"/>
+    <col min="4" max="16384" width="11.453125" style="35"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="13" x14ac:dyDescent="0.3">
+      <c r="A1" s="40" t="s">
+        <v>69</v>
+      </c>
+      <c r="B1" s="40" t="s">
+        <v>180</v>
+      </c>
+      <c r="C1" s="40" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="83" t="s">
+        <v>187</v>
+      </c>
+      <c r="B2" s="80" t="s">
+        <v>59</v>
+      </c>
+      <c r="C2" s="80"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="83" t="s">
+        <v>208</v>
+      </c>
+      <c r="B3" s="80" t="s">
+        <v>59</v>
+      </c>
+      <c r="C3" s="80"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="84" t="s">
+        <v>58</v>
+      </c>
+      <c r="B4" s="80" t="s">
+        <v>136</v>
+      </c>
+      <c r="C4" s="80"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="84" t="s">
+        <v>137</v>
+      </c>
+      <c r="B5" s="80" t="s">
+        <v>136</v>
+      </c>
+      <c r="C5" s="80"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="84"/>
+      <c r="B6" s="85"/>
+      <c r="C6" s="85"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="84"/>
+      <c r="B7" s="85"/>
+      <c r="C7" s="85"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="84"/>
+      <c r="B8" s="85"/>
+      <c r="C8" s="85"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="84"/>
+      <c r="B9" s="85"/>
+      <c r="C9" s="85"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="84"/>
+      <c r="B10" s="85"/>
+      <c r="C10" s="85"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="86"/>
+      <c r="B11" s="85"/>
+      <c r="C11" s="85"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="86"/>
+      <c r="B12" s="85"/>
+      <c r="C12" s="85"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="86"/>
+      <c r="B13" s="85"/>
+      <c r="C13" s="85"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="86"/>
+      <c r="B14" s="85"/>
+      <c r="C14" s="85"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="86"/>
+      <c r="B15" s="85"/>
+      <c r="C15" s="85"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="86"/>
+      <c r="B16" s="85"/>
+      <c r="C16" s="85"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="86"/>
+      <c r="B17" s="85"/>
+      <c r="C17" s="85"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="86"/>
+      <c r="B18" s="85"/>
+      <c r="C18" s="85"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="84"/>
+      <c r="B19" s="85"/>
+      <c r="C19" s="85"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="84"/>
+      <c r="B20" s="85"/>
+      <c r="C20" s="85"/>
+    </row>
+  </sheetData>
+  <sheetProtection algorithmName="SHA-512" hashValue="mJIhFbJiXwMDYdaTQpBnnIuyYOuT68NH0zRKA9hB05n6uZvdwWxrgEXuFwGJ+96DUDA/ASxdRlcLT7WZRHSmMg==" saltValue="bb4cIfhca5ee56tuIEArcQ==" spinCount="100000" sheet="1" scenarios="1" selectLockedCells="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -7349,7 +7363,7 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <sheetPr>
     <tabColor theme="0" tint="-0.249977111117893"/>
   </sheetPr>
@@ -7558,7 +7572,7 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <sheetPr>
     <tabColor theme="0" tint="-0.249977111117893"/>
   </sheetPr>
@@ -9327,7 +9341,7 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <sheetPr>
     <tabColor theme="0" tint="-0.249977111117893"/>
   </sheetPr>
@@ -10073,7 +10087,7 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <sheetPr>
     <tabColor theme="0" tint="-0.249977111117893"/>
   </sheetPr>
@@ -10447,7 +10461,7 @@
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
   <sheetPr>
     <tabColor theme="0" tint="-0.249977111117893"/>
   </sheetPr>
@@ -11564,6 +11578,12 @@
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="BiU9BXNF+INgNxSFtHuqKvDgOHy4i8LHe4WBopPE5oAPe1uu8rzbQfKL4uxCQ4dbx+6qcxc95feCcYk3II7eJw==" saltValue="oFkUqZTkt+d2Svo646TgPw==" spinCount="100000" sheet="1" scenarios="1" selectLockedCells="1"/>
   <mergeCells count="15">
+    <mergeCell ref="B19:B21"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="B14:B16"/>
     <mergeCell ref="B42:B44"/>
     <mergeCell ref="B45:B47"/>
     <mergeCell ref="B48:B50"/>
@@ -11573,12 +11593,6 @@
     <mergeCell ref="B31:B33"/>
     <mergeCell ref="B36:B38"/>
     <mergeCell ref="B39:B41"/>
-    <mergeCell ref="B19:B21"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="B5:B7"/>
-    <mergeCell ref="B8:B10"/>
-    <mergeCell ref="B11:B13"/>
-    <mergeCell ref="B14:B16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -11586,7 +11600,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <tabColor rgb="FF007600"/>
   </sheetPr>
@@ -12682,7 +12696,7 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
   <sheetPr>
     <tabColor theme="0" tint="-0.249977111117893"/>
   </sheetPr>
@@ -13079,13 +13093,13 @@
 </file>
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
   <sheetPr>
     <tabColor theme="0" tint="-0.249977111117893"/>
   </sheetPr>
   <dimension ref="A1:P111"/>
   <sheetViews>
-    <sheetView topLeftCell="A75" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A64" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
@@ -14569,7 +14583,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="56" spans="1:16" s="36" customFormat="1" ht="13" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:16" s="36" customFormat="1" ht="26" x14ac:dyDescent="0.3">
       <c r="A56" s="121" t="s">
         <v>70</v>
       </c>
@@ -15982,14 +15996,14 @@
 </file>
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
   <sheetPr>
     <tabColor theme="0" tint="-0.249977111117893"/>
   </sheetPr>
   <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -16292,14 +16306,14 @@
 </file>
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
   <sheetPr>
     <tabColor theme="0" tint="-0.249977111117893"/>
   </sheetPr>
   <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.08984375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -16375,10 +16389,10 @@
         <v>259</v>
       </c>
       <c r="C4" s="136">
-        <v>0.15</v>
+        <v>0</v>
       </c>
       <c r="D4" s="136">
-        <v>0.15</v>
+        <v>0</v>
       </c>
       <c r="E4" s="136">
         <v>0</v>
@@ -16413,10 +16427,10 @@
         <v>259</v>
       </c>
       <c r="C6" s="136">
-        <v>0.15</v>
+        <v>0</v>
       </c>
       <c r="D6" s="136">
-        <v>0.15</v>
+        <v>0</v>
       </c>
       <c r="E6" s="136">
         <v>0</v>
@@ -16571,14 +16585,14 @@
 </file>
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1700-000000000000}">
   <sheetPr>
     <tabColor theme="0" tint="-0.249977111117893"/>
   </sheetPr>
   <dimension ref="A1:O28"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E20" sqref="E20:O20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -17314,37 +17328,37 @@
         <v>1</v>
       </c>
       <c r="E20" s="136">
-        <v>0.9</v>
+        <v>0.97599999999999998</v>
       </c>
       <c r="F20" s="136">
-        <v>0.9</v>
+        <v>0.97599999999999998</v>
       </c>
       <c r="G20" s="136">
-        <v>0.9</v>
+        <v>0.97599999999999998</v>
       </c>
       <c r="H20" s="136">
-        <v>0.9</v>
+        <v>0.97599999999999998</v>
       </c>
       <c r="I20" s="136">
-        <v>0.9</v>
+        <v>0.97599999999999998</v>
       </c>
       <c r="J20" s="136">
-        <v>0.9</v>
+        <v>0.97599999999999998</v>
       </c>
       <c r="K20" s="136">
-        <v>0.9</v>
+        <v>0.97599999999999998</v>
       </c>
       <c r="L20" s="136">
-        <v>0.9</v>
+        <v>0.97599999999999998</v>
       </c>
       <c r="M20" s="136">
-        <v>0.9</v>
+        <v>0.97599999999999998</v>
       </c>
       <c r="N20" s="136">
-        <v>0.9</v>
+        <v>0.97599999999999998</v>
       </c>
       <c r="O20" s="136">
-        <v>0.9</v>
+        <v>0.97599999999999998</v>
       </c>
     </row>
     <row r="25" spans="2:15" x14ac:dyDescent="0.25">
@@ -17367,14 +17381,14 @@
 </file>
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1800-000000000000}">
   <sheetPr>
     <tabColor theme="0" tint="-0.249977111117893"/>
   </sheetPr>
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="D3" sqref="D3:G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -17417,16 +17431,16 @@
         <v>1</v>
       </c>
       <c r="D3" s="136">
-        <v>0.21</v>
+        <v>0.22</v>
       </c>
       <c r="E3" s="136">
-        <v>0.21</v>
+        <v>0.22</v>
       </c>
       <c r="F3" s="136">
-        <v>0.21</v>
+        <v>0.22</v>
       </c>
       <c r="G3" s="136">
-        <v>0.21</v>
+        <v>0.22</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="13" x14ac:dyDescent="0.3">
@@ -17448,16 +17462,16 @@
         <v>1</v>
       </c>
       <c r="D5" s="136">
-        <v>0.14299999999999999</v>
+        <v>0.16</v>
       </c>
       <c r="E5" s="136">
-        <v>0.14299999999999999</v>
+        <v>0.16</v>
       </c>
       <c r="F5" s="136">
-        <v>0.14299999999999999</v>
+        <v>0.16</v>
       </c>
       <c r="G5" s="136">
-        <v>0.14299999999999999</v>
+        <v>0.16</v>
       </c>
     </row>
   </sheetData>
@@ -17468,14 +17482,14 @@
 </file>
 
 <file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1900-000000000000}">
   <sheetPr>
     <tabColor theme="0" tint="-0.249977111117893"/>
   </sheetPr>
   <dimension ref="A1:I49"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" zoomScale="111" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView topLeftCell="A2" zoomScale="111" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -17554,13 +17568,13 @@
         <v>0</v>
       </c>
       <c r="F3" s="136">
-        <v>0.53134328358208949</v>
+        <v>0.36</v>
       </c>
       <c r="G3" s="136">
-        <v>0.53134328358208949</v>
+        <v>0.36</v>
       </c>
       <c r="H3" s="136">
-        <v>0.53134328358208949</v>
+        <v>0.36</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -17574,13 +17588,13 @@
         <v>0</v>
       </c>
       <c r="F4" s="136">
-        <v>0.38507462686567184</v>
+        <v>0.45</v>
       </c>
       <c r="G4" s="136">
-        <v>0.38507462686567184</v>
+        <v>0.45</v>
       </c>
       <c r="H4" s="136">
-        <v>0.38507462686567184</v>
+        <v>0.45</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -17663,7 +17677,7 @@
         <v>0</v>
       </c>
       <c r="F8" s="136">
-        <v>0.25970149253731345</v>
+        <v>0.25970149253731301</v>
       </c>
       <c r="G8" s="136">
         <v>0.25970149253731345</v>
@@ -17778,13 +17792,13 @@
         <v>0</v>
       </c>
       <c r="F13" s="136">
-        <v>0.33500000000000002</v>
+        <v>0.8</v>
       </c>
       <c r="G13" s="136">
-        <v>0.33500000000000002</v>
+        <v>0.8</v>
       </c>
       <c r="H13" s="136">
-        <v>0.33500000000000002</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -17798,13 +17812,13 @@
         <v>0</v>
       </c>
       <c r="F14" s="136">
-        <v>0.7</v>
+        <v>0.85</v>
       </c>
       <c r="G14" s="136">
-        <v>0.62</v>
+        <v>0.85</v>
       </c>
       <c r="H14" s="136">
-        <v>0.62</v>
+        <v>0.85</v>
       </c>
       <c r="I14" s="36"/>
     </row>
@@ -17822,13 +17836,13 @@
         <v>0</v>
       </c>
       <c r="F15" s="136">
-        <v>0.33500000000000002</v>
+        <v>0.8</v>
       </c>
       <c r="G15" s="136">
-        <v>0.33500000000000002</v>
+        <v>0.8</v>
       </c>
       <c r="H15" s="136">
-        <v>0.33500000000000002</v>
+        <v>0.8</v>
       </c>
       <c r="I15" s="36"/>
     </row>
@@ -17843,13 +17857,13 @@
         <v>0</v>
       </c>
       <c r="F16" s="136">
-        <v>0.84</v>
+        <v>0.75</v>
       </c>
       <c r="G16" s="136">
-        <v>0.62</v>
+        <v>0.75</v>
       </c>
       <c r="H16" s="136">
-        <v>0.62</v>
+        <v>0.75</v>
       </c>
       <c r="I16" s="36"/>
     </row>
@@ -17885,7 +17899,7 @@
         <v>268</v>
       </c>
       <c r="D18" s="136">
-        <v>0.46</v>
+        <v>0.186</v>
       </c>
       <c r="E18" s="136">
         <v>0</v>
@@ -17932,7 +17946,7 @@
         <v>268</v>
       </c>
       <c r="D20" s="136">
-        <v>0.46</v>
+        <v>0.186</v>
       </c>
       <c r="E20" s="136">
         <v>0</v>
@@ -17978,7 +17992,7 @@
         <v>268</v>
       </c>
       <c r="D22" s="136">
-        <v>0.46</v>
+        <v>0.186</v>
       </c>
       <c r="E22" s="136">
         <v>0</v>
@@ -18354,19 +18368,19 @@
         <v>268</v>
       </c>
       <c r="D39" s="136">
-        <v>0.5</v>
+        <v>0.6</v>
       </c>
       <c r="E39" s="136">
-        <v>0.5</v>
+        <v>0.6</v>
       </c>
       <c r="F39" s="136">
-        <v>0.5</v>
+        <v>0.6</v>
       </c>
       <c r="G39" s="136">
-        <v>0.5</v>
+        <v>0.6</v>
       </c>
       <c r="H39" s="136">
-        <v>0.5</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
@@ -18374,19 +18388,19 @@
         <v>269</v>
       </c>
       <c r="D40" s="136">
-        <v>0.65</v>
+        <v>0.45</v>
       </c>
       <c r="E40" s="136">
-        <v>0.65</v>
+        <v>0.45</v>
       </c>
       <c r="F40" s="136">
-        <v>0.65</v>
+        <v>0.45</v>
       </c>
       <c r="G40" s="136">
-        <v>0.65</v>
+        <v>0.45</v>
       </c>
       <c r="H40" s="136">
-        <v>0.65</v>
+        <v>0.45</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
@@ -18417,19 +18431,19 @@
         <v>268</v>
       </c>
       <c r="D42" s="136">
-        <v>0.49</v>
+        <v>0.5</v>
       </c>
       <c r="E42" s="136">
-        <v>0.49</v>
+        <v>0.5</v>
       </c>
       <c r="F42" s="136">
-        <v>0.49</v>
+        <v>0.5</v>
       </c>
       <c r="G42" s="136">
-        <v>0.49</v>
+        <v>0.5</v>
       </c>
       <c r="H42" s="136">
-        <v>0.49</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
@@ -18437,19 +18451,19 @@
         <v>269</v>
       </c>
       <c r="D43" s="136">
-        <v>0.52</v>
+        <v>0.63</v>
       </c>
       <c r="E43" s="136">
-        <v>0.52</v>
+        <v>0.63</v>
       </c>
       <c r="F43" s="136">
-        <v>0.52</v>
+        <v>0.63</v>
       </c>
       <c r="G43" s="136">
-        <v>0.52</v>
+        <v>0.63</v>
       </c>
       <c r="H43" s="136">
-        <v>0.52</v>
+        <v>0.63</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
@@ -18483,19 +18497,19 @@
         <v>268</v>
       </c>
       <c r="D45" s="136">
-        <v>0.93</v>
+        <v>0.8</v>
       </c>
       <c r="E45" s="136">
-        <v>0.93</v>
+        <v>0.8</v>
       </c>
       <c r="F45" s="136">
-        <v>0.93</v>
+        <v>0.8</v>
       </c>
       <c r="G45" s="136">
-        <v>0.93</v>
+        <v>0.8</v>
       </c>
       <c r="H45" s="136">
-        <v>0.93</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
@@ -18529,19 +18543,19 @@
         <v>268</v>
       </c>
       <c r="D47" s="136">
-        <v>0.86</v>
+        <v>0.76</v>
       </c>
       <c r="E47" s="136">
-        <v>0.86</v>
+        <v>0.76</v>
       </c>
       <c r="F47" s="136">
-        <v>0.86</v>
+        <v>0.76</v>
       </c>
       <c r="G47" s="136">
-        <v>0.86</v>
+        <v>0.76</v>
       </c>
       <c r="H47" s="136">
-        <v>0.86</v>
+        <v>0.76</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
@@ -18558,7 +18572,7 @@
         <v>0.57999999999999996</v>
       </c>
       <c r="E48" s="136">
-        <v>0.57999999999999996</v>
+        <v>0</v>
       </c>
       <c r="F48" s="136">
         <v>0</v>
@@ -18575,10 +18589,10 @@
         <v>268</v>
       </c>
       <c r="D49" s="136">
-        <v>0.51</v>
+        <v>0.88</v>
       </c>
       <c r="E49" s="136">
-        <v>0.51</v>
+        <v>0</v>
       </c>
       <c r="F49" s="136">
         <v>0</v>
@@ -18598,14 +18612,14 @@
 </file>
 
 <file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1A00-000000000000}">
   <sheetPr>
     <tabColor theme="0" tint="-0.249977111117893"/>
   </sheetPr>
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -18754,16 +18768,16 @@
         <v>268</v>
       </c>
       <c r="D7" s="136">
-        <v>0.6</v>
+        <v>0.59</v>
       </c>
       <c r="E7" s="136">
-        <v>0.6</v>
+        <v>0.59</v>
       </c>
       <c r="F7" s="136">
-        <v>0.6</v>
+        <v>0.59</v>
       </c>
       <c r="G7" s="136">
-        <v>0.6</v>
+        <v>0.59</v>
       </c>
       <c r="H7" s="128"/>
     </row>
@@ -18774,7 +18788,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <tabColor rgb="FF007600"/>
   </sheetPr>
@@ -19213,7 +19227,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <tabColor rgb="FF007600"/>
   </sheetPr>
@@ -19287,23 +19301,23 @@
         <v>118</v>
       </c>
       <c r="C3" s="76">
-        <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(C4:C5), 0, 1) + 1, 0, 1, TRUE) - _xlfn.SUM(C4:C5), "")</f>
+        <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(C4:C5), 0, 1) + 1, 0, 1, TRUE) - SUM(C4:C5), "")</f>
         <v>0.32228430019523346</v>
       </c>
       <c r="D3" s="76">
-        <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(D4:D5), 0, 1) + 1, 0, 1, TRUE) - _xlfn.SUM(D4:D5), "")</f>
+        <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(D4:D5), 0, 1) + 1, 0, 1, TRUE) - SUM(D4:D5), "")</f>
         <v>0.32228430019523346</v>
       </c>
       <c r="E3" s="76">
-        <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(E4:E5), 0, 1) + 1, 0, 1, TRUE) - _xlfn.SUM(E4:E5), "")</f>
+        <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(E4:E5), 0, 1) + 1, 0, 1, TRUE) - SUM(E4:E5), "")</f>
         <v>0.35908666207150708</v>
       </c>
       <c r="F3" s="76">
-        <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(F4:F5), 0, 1) + 1, 0, 1, TRUE) - _xlfn.SUM(F4:F5), "")</f>
+        <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(F4:F5), 0, 1) + 1, 0, 1, TRUE) - SUM(F4:F5), "")</f>
         <v>0.37651189492768178</v>
       </c>
       <c r="G3" s="76">
-        <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(G4:G5), 0, 1) + 1, 0, 1, TRUE) - _xlfn.SUM(G4:G5), "")</f>
+        <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(G4:G5), 0, 1) + 1, 0, 1, TRUE) - SUM(G4:G5), "")</f>
         <v>0.37372365733745416</v>
       </c>
     </row>
@@ -19398,23 +19412,23 @@
         <v>121</v>
       </c>
       <c r="C9" s="76">
-        <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(C10:C11), 0, 1) + 1, 0, 1, TRUE) - _xlfn.SUM(C10:C11), "")</f>
+        <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(C10:C11), 0, 1) + 1, 0, 1, TRUE) - SUM(C10:C11), "")</f>
         <v>0.28180440984664923</v>
       </c>
       <c r="D9" s="76">
-        <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(D10:D11), 0, 1) + 1, 0, 1, TRUE) - _xlfn.SUM(D10:D11), "")</f>
+        <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(D10:D11), 0, 1) + 1, 0, 1, TRUE) - SUM(D10:D11), "")</f>
         <v>0.28180440984664923</v>
       </c>
       <c r="E9" s="76">
-        <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(E10:E11), 0, 1) + 1, 0, 1, TRUE) - _xlfn.SUM(E10:E11), "")</f>
+        <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(E10:E11), 0, 1) + 1, 0, 1, TRUE) - SUM(E10:E11), "")</f>
         <v>0.2466938696379041</v>
       </c>
       <c r="F9" s="76">
-        <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(F10:F11), 0, 1) + 1, 0, 1, TRUE) - _xlfn.SUM(F10:F11), "")</f>
+        <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(F10:F11), 0, 1) + 1, 0, 1, TRUE) - SUM(F10:F11), "")</f>
         <v>0.21506846670192739</v>
       </c>
       <c r="G9" s="76">
-        <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(G10:G11), 0, 1) + 1, 0, 1, TRUE) - _xlfn.SUM(G10:G11), "")</f>
+        <f>IFERROR(_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(G10:G11), 0, 1) + 1, 0, 1, TRUE) - SUM(G10:G11), "")</f>
         <v>0.15821429221536368</v>
       </c>
     </row>
@@ -19640,7 +19654,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr>
     <tabColor rgb="FF007600"/>
   </sheetPr>
@@ -19776,13 +19790,13 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr>
     <tabColor rgb="FF007600"/>
   </sheetPr>
   <dimension ref="A1:P14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView topLeftCell="C1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
@@ -20091,7 +20105,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <sheetPr>
     <tabColor theme="7" tint="-0.249977111117893"/>
   </sheetPr>
@@ -20367,7 +20381,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <sheetPr>
     <tabColor theme="7" tint="-0.249977111117893"/>
   </sheetPr>
@@ -20430,7 +20444,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <sheetPr>
     <tabColor theme="7" tint="-0.249977111117893"/>
   </sheetPr>
@@ -21103,7 +21117,7 @@
     </row>
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="jSdherlZJbZ8Sy1L59bo9v5QauB4K+9LWnSRVPNbXJxTAgxgiv9ErxgnISHZ2apMgabDAJDnLmaWIXWQOwB0iA==" saltValue="GDpAVnNFn9RTLmsUAjB9Mw==" spinCount="100000" sheet="1" scenarios="1" selectLockedCells="1"/>
-  <sortState ref="A2:D38">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D38">
     <sortCondition ref="A2:A38"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -21112,7 +21126,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0800-000000000000}">
           <x14:formula1>
             <xm:f>'Cost curve options'!$A$1:$A$4</xm:f>
           </x14:formula1>

</xml_diff>

<commit_message>
Fix to geospatial allocations
</commit_message>
<xml_diff>
--- a/inputs/demo_demo_input.xlsx
+++ b/inputs/demo_demo_input.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22827"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dominic.delport\Documents\GitHub\Nutrition\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3A74EB16-E57F-43FD-989D-00DC64EFA992}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDB4B1E4-D389-4670-BF20-494694F50BBA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-80" yWindow="-80" windowWidth="19360" windowHeight="10360" tabRatio="885" firstSheet="6" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="885" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Baseline year population inputs" sheetId="1" r:id="rId1"/>
@@ -465,7 +465,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1092" uniqueCount="270">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1095" uniqueCount="272">
   <si>
     <t>year</t>
   </si>
@@ -1275,6 +1275,12 @@
   </si>
   <si>
     <t>Effectiveness incidence</t>
+  </si>
+  <si>
+    <t>Prevalence of pre-eclampsia</t>
+  </si>
+  <si>
+    <t>Prevalence of eclampsia</t>
   </si>
 </sst>
 </file>
@@ -4799,8 +4805,8 @@
   </sheetPr>
   <dimension ref="A1:E63"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -5239,11 +5245,27 @@
         <v>0.42</v>
       </c>
     </row>
+    <row r="60" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B60" s="16" t="s">
+        <v>270</v>
+      </c>
+      <c r="C60" s="66">
+        <v>4.5999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B61" s="16" t="s">
+        <v>271</v>
+      </c>
+      <c r="C61" s="66">
+        <v>1.4E-2</v>
+      </c>
+    </row>
     <row r="63" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A63" s="4"/>
     </row>
   </sheetData>
-  <sheetProtection password="CA9F" sheet="1" scenarios="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="Fe3O/MXXtRaxGdMonYb1nwe/aLwU7VpdYcsmQcLBypCxbjEhlBLAvV27SVO87s23lMfP3pbK5a6p6d5Q5jn+Cg==" saltValue="v5slMoMRZDGvHohUBj+cCg==" spinCount="100000" sheet="1" scenarios="1" selectLockedCells="1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
 </worksheet>
@@ -7187,7 +7209,7 @@
   </sheetPr>
   <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -11578,12 +11600,6 @@
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="BiU9BXNF+INgNxSFtHuqKvDgOHy4i8LHe4WBopPE5oAPe1uu8rzbQfKL4uxCQ4dbx+6qcxc95feCcYk3II7eJw==" saltValue="oFkUqZTkt+d2Svo646TgPw==" spinCount="100000" sheet="1" scenarios="1" selectLockedCells="1"/>
   <mergeCells count="15">
-    <mergeCell ref="B19:B21"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="B5:B7"/>
-    <mergeCell ref="B8:B10"/>
-    <mergeCell ref="B11:B13"/>
-    <mergeCell ref="B14:B16"/>
     <mergeCell ref="B42:B44"/>
     <mergeCell ref="B45:B47"/>
     <mergeCell ref="B48:B50"/>
@@ -11593,6 +11609,12 @@
     <mergeCell ref="B31:B33"/>
     <mergeCell ref="B36:B38"/>
     <mergeCell ref="B39:B41"/>
+    <mergeCell ref="B19:B21"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="B14:B16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -20112,7 +20134,7 @@
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -20290,7 +20312,9 @@
       </c>
       <c r="C14" s="45"/>
       <c r="D14" s="44"/>
-      <c r="E14" s="80"/>
+      <c r="E14" s="80" t="s">
+        <v>194</v>
+      </c>
     </row>
     <row r="16" spans="1:5" ht="13" x14ac:dyDescent="0.3">
       <c r="A16" s="49" t="s">

</xml_diff>

<commit_message>
Update unit cost heading in programs cost and coverage sheet
</commit_message>
<xml_diff>
--- a/inputs/demo_demo_input.xlsx
+++ b/inputs/demo_demo_input.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dominic.delport\Documents\GitHub\Nutrition\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDB4B1E4-D389-4670-BF20-494694F50BBA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57666FFC-B104-448E-A4B3-04EB8EFAD0C2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="885" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="885" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Baseline year population inputs" sheetId="1" r:id="rId1"/>
@@ -1085,9 +1085,6 @@
     <t>Cost-coverage relationship</t>
   </si>
   <si>
-    <t>Unit cost (US$ per person per year)</t>
-  </si>
-  <si>
     <t>IFAS (health facility)</t>
   </si>
   <si>
@@ -1281,6 +1278,9 @@
   </si>
   <si>
     <t>Prevalence of eclampsia</t>
+  </si>
+  <si>
+    <t>Unit cost (US$)</t>
   </si>
 </sst>
 </file>
@@ -4805,7 +4805,7 @@
   </sheetPr>
   <dimension ref="A1:E63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
@@ -4864,7 +4864,7 @@
     </row>
     <row r="7" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="16" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C7" s="65">
         <v>9862402</v>
@@ -5247,7 +5247,7 @@
     </row>
     <row r="60" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B60" s="16" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C60" s="66">
         <v>4.5999999999999999E-2</v>
@@ -5255,7 +5255,7 @@
     </row>
     <row r="61" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B61" s="16" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C61" s="66">
         <v>1.4E-2</v>
@@ -6216,7 +6216,7 @@
     <row r="17" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="4"/>
       <c r="B17" s="11" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C17" s="88">
         <v>0</v>
@@ -6550,7 +6550,7 @@
     </row>
     <row r="25" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="59" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C25" s="88">
         <v>0</v>
@@ -7243,7 +7243,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="83" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B3" s="80" t="s">
         <v>59</v>
@@ -8437,7 +8437,7 @@
     </row>
     <row r="20" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B20" s="90" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C20" s="133">
         <v>0</v>
@@ -8766,7 +8766,7 @@
     <row r="28" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="56"/>
       <c r="B28" s="59" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C28" s="133">
         <v>0</v>
@@ -9393,16 +9393,16 @@
         <v>69</v>
       </c>
       <c r="B1" s="35" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C1" s="35" t="s">
         <v>70</v>
       </c>
       <c r="D1" s="35" t="s">
+        <v>212</v>
+      </c>
+      <c r="E1" s="35" t="s">
         <v>213</v>
-      </c>
-      <c r="E1" s="35" t="s">
-        <v>214</v>
       </c>
       <c r="F1" s="35" t="s">
         <v>24</v>
@@ -9414,13 +9414,13 @@
         <v>74</v>
       </c>
       <c r="I1" s="35" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="J1" s="35" t="s">
         <v>196</v>
       </c>
       <c r="K1" s="35" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -9586,7 +9586,7 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="59" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B11" s="133"/>
       <c r="C11" s="133" t="s">
@@ -9656,7 +9656,7 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="90" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B15" s="133"/>
       <c r="C15" s="133" t="s">
@@ -10136,19 +10136,19 @@
   <sheetData>
     <row r="1" spans="1:11" ht="13" x14ac:dyDescent="0.3">
       <c r="A1" s="40" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B1" s="35" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C1" s="35" t="s">
         <v>70</v>
       </c>
       <c r="D1" s="35" t="s">
+        <v>212</v>
+      </c>
+      <c r="E1" s="35" t="s">
         <v>213</v>
-      </c>
-      <c r="E1" s="35" t="s">
-        <v>214</v>
       </c>
       <c r="F1" s="35" t="s">
         <v>24</v>
@@ -10160,13 +10160,13 @@
         <v>74</v>
       </c>
       <c r="I1" s="35" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="J1" s="35" t="s">
         <v>196</v>
       </c>
       <c r="K1" s="35" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -10503,7 +10503,7 @@
   <sheetData>
     <row r="1" spans="1:10" ht="13" x14ac:dyDescent="0.3">
       <c r="A1" s="40" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B1" s="40" t="s">
         <v>177</v>
@@ -10529,7 +10529,7 @@
     </row>
     <row r="2" spans="1:10" ht="13" x14ac:dyDescent="0.3">
       <c r="A2" s="40" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B2" s="137" t="s">
         <v>32</v>
@@ -10890,7 +10890,7 @@
     </row>
     <row r="19" spans="1:8" ht="13" x14ac:dyDescent="0.3">
       <c r="A19" s="40" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B19" s="137" t="s">
         <v>32</v>
@@ -11248,7 +11248,7 @@
     </row>
     <row r="36" spans="1:8" ht="13" x14ac:dyDescent="0.3">
       <c r="A36" s="97" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B36" s="137" t="s">
         <v>32</v>
@@ -11600,6 +11600,12 @@
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="BiU9BXNF+INgNxSFtHuqKvDgOHy4i8LHe4WBopPE5oAPe1uu8rzbQfKL4uxCQ4dbx+6qcxc95feCcYk3II7eJw==" saltValue="oFkUqZTkt+d2Svo646TgPw==" spinCount="100000" sheet="1" scenarios="1" selectLockedCells="1"/>
   <mergeCells count="15">
+    <mergeCell ref="B19:B21"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="B14:B16"/>
     <mergeCell ref="B42:B44"/>
     <mergeCell ref="B45:B47"/>
     <mergeCell ref="B48:B50"/>
@@ -11609,12 +11615,6 @@
     <mergeCell ref="B31:B33"/>
     <mergeCell ref="B36:B38"/>
     <mergeCell ref="B39:B41"/>
-    <mergeCell ref="B19:B21"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="B5:B7"/>
-    <mergeCell ref="B8:B10"/>
-    <mergeCell ref="B11:B13"/>
-    <mergeCell ref="B14:B16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -12740,7 +12740,7 @@
   <sheetData>
     <row r="1" spans="1:7" s="100" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="99" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -12760,7 +12760,7 @@
     </row>
     <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="40" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B3" s="104"/>
       <c r="C3" s="105"/>
@@ -12844,7 +12844,7 @@
     </row>
     <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="40" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C9" s="135">
         <v>1</v>
@@ -12869,7 +12869,7 @@
     </row>
     <row r="11" spans="1:7" s="100" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="99" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C11" s="110"/>
       <c r="D11" s="111"/>
@@ -12879,7 +12879,7 @@
     </row>
     <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="40" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C12" s="108"/>
       <c r="D12" s="95"/>
@@ -12889,7 +12889,7 @@
     </row>
     <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="113" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C13" s="135">
         <v>1</v>
@@ -12907,7 +12907,7 @@
     </row>
     <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="113" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C14" s="135">
         <v>1</v>
@@ -12925,7 +12925,7 @@
     </row>
     <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="113" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C15" s="135">
         <v>1</v>
@@ -12952,7 +12952,7 @@
     </row>
     <row r="17" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="40" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B17" s="104"/>
       <c r="C17" s="115"/>
@@ -13138,18 +13138,18 @@
   <sheetData>
     <row r="1" spans="1:16" s="100" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A1" s="99" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="2" spans="1:16" ht="13" x14ac:dyDescent="0.3">
       <c r="A2" s="118" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B2" s="119" t="s">
+        <v>231</v>
+      </c>
+      <c r="C2" s="119" t="s">
         <v>232</v>
-      </c>
-      <c r="C2" s="119" t="s">
-        <v>233</v>
       </c>
       <c r="D2" s="103" t="s">
         <v>1</v>
@@ -13181,7 +13181,7 @@
         <v>71</v>
       </c>
       <c r="C3" s="43" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D3" s="135">
         <v>1</v>
@@ -13209,7 +13209,7 @@
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C4" s="43" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D4" s="136">
         <v>1</v>
@@ -13237,7 +13237,7 @@
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C5" s="43" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D5" s="136">
         <v>1</v>
@@ -13265,7 +13265,7 @@
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C6" s="43" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D6" s="136">
         <v>1</v>
@@ -13296,7 +13296,7 @@
         <v>16</v>
       </c>
       <c r="C7" s="43" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D7" s="135">
         <v>1</v>
@@ -13324,7 +13324,7 @@
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C8" s="43" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D8" s="136">
         <v>1</v>
@@ -13352,7 +13352,7 @@
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C9" s="43" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D9" s="136">
         <v>1</v>
@@ -13380,7 +13380,7 @@
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C10" s="43" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D10" s="136">
         <v>1</v>
@@ -13411,7 +13411,7 @@
         <v>18</v>
       </c>
       <c r="C11" s="43" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D11" s="135">
         <v>1</v>
@@ -13439,7 +13439,7 @@
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C12" s="43" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D12" s="136">
         <v>1</v>
@@ -13467,7 +13467,7 @@
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C13" s="43" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D13" s="136">
         <v>1</v>
@@ -13495,7 +13495,7 @@
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C14" s="43" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D14" s="136">
         <v>1</v>
@@ -13526,7 +13526,7 @@
         <v>19</v>
       </c>
       <c r="C15" s="43" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D15" s="135">
         <v>1</v>
@@ -13554,7 +13554,7 @@
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C16" s="43" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D16" s="136">
         <v>1</v>
@@ -13582,7 +13582,7 @@
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C17" s="43" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D17" s="136">
         <v>1</v>
@@ -13610,7 +13610,7 @@
     </row>
     <row r="18" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C18" s="43" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D18" s="136">
         <v>1</v>
@@ -13641,7 +13641,7 @@
         <v>17</v>
       </c>
       <c r="C19" s="43" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D19" s="135">
         <v>1</v>
@@ -13669,7 +13669,7 @@
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C20" s="43" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D20" s="136">
         <v>1</v>
@@ -13697,7 +13697,7 @@
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C21" s="43" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D21" s="136">
         <v>1</v>
@@ -13725,7 +13725,7 @@
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C22" s="43" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D22" s="136">
         <v>1</v>
@@ -13756,7 +13756,7 @@
         <v>23</v>
       </c>
       <c r="C23" s="43" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D23" s="135">
         <v>1</v>
@@ -13784,7 +13784,7 @@
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C24" s="43" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D24" s="136">
         <v>1</v>
@@ -13812,7 +13812,7 @@
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C25" s="43" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D25" s="136">
         <v>1</v>
@@ -13840,7 +13840,7 @@
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C26" s="43" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D26" s="136">
         <v>1</v>
@@ -13868,18 +13868,18 @@
     </row>
     <row r="28" spans="1:16" s="100" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A28" s="99" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="29" spans="1:16" s="36" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A29" s="121" t="s">
+        <v>238</v>
+      </c>
+      <c r="B29" s="94" t="s">
+        <v>231</v>
+      </c>
+      <c r="C29" s="94" t="s">
         <v>239</v>
-      </c>
-      <c r="B29" s="94" t="s">
-        <v>232</v>
-      </c>
-      <c r="C29" s="94" t="s">
-        <v>240</v>
       </c>
       <c r="D29" s="103" t="s">
         <v>1</v>
@@ -13911,7 +13911,7 @@
         <v>71</v>
       </c>
       <c r="C30" s="43" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D30" s="135">
         <v>1</v>
@@ -13939,7 +13939,7 @@
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C31" s="43" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D31" s="136">
         <v>1</v>
@@ -14026,7 +14026,7 @@
         <v>16</v>
       </c>
       <c r="C34" s="43" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D34" s="135">
         <v>1</v>
@@ -14054,7 +14054,7 @@
     </row>
     <row r="35" spans="2:16" x14ac:dyDescent="0.25">
       <c r="C35" s="43" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D35" s="136">
         <v>1</v>
@@ -14141,7 +14141,7 @@
         <v>18</v>
       </c>
       <c r="C38" s="43" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D38" s="135">
         <v>1</v>
@@ -14169,7 +14169,7 @@
     </row>
     <row r="39" spans="2:16" x14ac:dyDescent="0.25">
       <c r="C39" s="43" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D39" s="136">
         <v>1</v>
@@ -14256,7 +14256,7 @@
         <v>19</v>
       </c>
       <c r="C42" s="43" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D42" s="135">
         <v>1</v>
@@ -14284,7 +14284,7 @@
     </row>
     <row r="43" spans="2:16" x14ac:dyDescent="0.25">
       <c r="C43" s="43" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D43" s="136">
         <v>1</v>
@@ -14371,7 +14371,7 @@
         <v>17</v>
       </c>
       <c r="C46" s="43" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D46" s="135">
         <v>1</v>
@@ -14399,7 +14399,7 @@
     </row>
     <row r="47" spans="2:16" x14ac:dyDescent="0.25">
       <c r="C47" s="43" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D47" s="136">
         <v>1</v>
@@ -14486,7 +14486,7 @@
         <v>23</v>
       </c>
       <c r="C50" s="43" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D50" s="135">
         <v>1</v>
@@ -14514,7 +14514,7 @@
     </row>
     <row r="51" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C51" s="43" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D51" s="136">
         <v>1</v>
@@ -14602,7 +14602,7 @@
     </row>
     <row r="55" spans="1:16" s="100" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A55" s="99" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="56" spans="1:16" s="36" customFormat="1" ht="26" x14ac:dyDescent="0.3">
@@ -14610,10 +14610,10 @@
         <v>70</v>
       </c>
       <c r="B56" s="94" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C56" s="123" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D56" s="103" t="s">
         <v>53</v>
@@ -14639,7 +14639,7 @@
         <v>38</v>
       </c>
       <c r="C57" s="43" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D57" s="135">
         <v>1</v>
@@ -14661,7 +14661,7 @@
     </row>
     <row r="58" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C58" s="43" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D58" s="136">
         <v>10.675000000000001</v>
@@ -14686,7 +14686,7 @@
         <v>39</v>
       </c>
       <c r="C59" s="43" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D59" s="135">
         <v>1</v>
@@ -14708,7 +14708,7 @@
     </row>
     <row r="60" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C60" s="43" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D60" s="136">
         <v>10.675000000000001</v>
@@ -14733,7 +14733,7 @@
         <v>40</v>
       </c>
       <c r="C61" s="43" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D61" s="135">
         <v>1</v>
@@ -14755,7 +14755,7 @@
     </row>
     <row r="62" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C62" s="43" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D62" s="136">
         <v>10.675000000000001</v>
@@ -14781,7 +14781,7 @@
     </row>
     <row r="64" spans="1:16" s="100" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A64" s="99" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="65" spans="1:16" s="36" customFormat="1" ht="26" x14ac:dyDescent="0.3">
@@ -14789,10 +14789,10 @@
         <v>24</v>
       </c>
       <c r="B65" s="94" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C65" s="123" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D65" s="103" t="s">
         <v>1</v>
@@ -15856,7 +15856,7 @@
     </row>
     <row r="103" spans="1:16" s="100" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A103" s="99" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="104" spans="1:16" s="36" customFormat="1" ht="26" x14ac:dyDescent="0.3">
@@ -15867,7 +15867,7 @@
         <v>169</v>
       </c>
       <c r="C104" s="123" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D104" s="103" t="s">
         <v>1</v>
@@ -16042,7 +16042,7 @@
   <sheetData>
     <row r="1" spans="1:7" s="100" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="99" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -16068,10 +16068,10 @@
     </row>
     <row r="3" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="113" t="s">
+        <v>248</v>
+      </c>
+      <c r="C3" s="136" t="s">
         <v>249</v>
-      </c>
-      <c r="C3" s="136" t="s">
-        <v>250</v>
       </c>
       <c r="D3" s="136">
         <v>45</v>
@@ -16089,7 +16089,7 @@
     <row r="4" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="40"/>
       <c r="B4" s="117" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C4" s="136">
         <v>1.0249999999999999</v>
@@ -16109,7 +16109,7 @@
     </row>
     <row r="5" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="104" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -16182,7 +16182,7 @@
     </row>
     <row r="10" spans="1:7" s="100" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="99" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -16212,15 +16212,15 @@
     </row>
     <row r="13" spans="1:7" s="100" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="99" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="125" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B14" s="117" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C14" s="136">
         <v>1.0249999999999999</v>
@@ -16241,7 +16241,7 @@
     <row r="15" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="40"/>
       <c r="B15" s="117" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C15" s="136">
         <v>1.0249999999999999</v>
@@ -16264,7 +16264,7 @@
         <v>70</v>
       </c>
       <c r="B16" s="113" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C16" s="136">
         <v>1</v>
@@ -16285,7 +16285,7 @@
     <row r="17" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="18" spans="1:6" s="100" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="99" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="19" spans="1:6" s="104" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -16370,7 +16370,7 @@
         <v>29</v>
       </c>
       <c r="B2" s="90" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C2" s="136">
         <v>0.21</v>
@@ -16388,7 +16388,7 @@
     <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="90"/>
       <c r="B3" s="90" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C3" s="136">
         <v>1</v>
@@ -16408,7 +16408,7 @@
         <v>187</v>
       </c>
       <c r="B4" s="90" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C4" s="136">
         <v>0</v>
@@ -16426,7 +16426,7 @@
     <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="90"/>
       <c r="B5" s="90" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C5" s="136">
         <v>1</v>
@@ -16443,10 +16443,10 @@
     </row>
     <row r="6" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="90" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B6" s="90" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C6" s="136">
         <v>0</v>
@@ -16464,7 +16464,7 @@
     <row r="7" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="90"/>
       <c r="B7" s="90" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C7" s="136">
         <v>1</v>
@@ -16484,7 +16484,7 @@
         <v>57</v>
       </c>
       <c r="B8" s="90" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C8" s="136">
         <v>0.35</v>
@@ -16502,7 +16502,7 @@
     <row r="9" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="90"/>
       <c r="B9" s="90" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C9" s="136">
         <v>1</v>
@@ -16522,7 +16522,7 @@
         <v>34</v>
       </c>
       <c r="B10" s="90" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C10" s="136">
         <v>0.35</v>
@@ -16540,7 +16540,7 @@
     <row r="11" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="90"/>
       <c r="B11" s="90" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C11" s="136">
         <v>1</v>
@@ -16560,7 +16560,7 @@
         <v>59</v>
       </c>
       <c r="B12" s="90" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C12" s="136">
         <v>0.08</v>
@@ -16578,7 +16578,7 @@
     <row r="13" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="90"/>
       <c r="B13" s="90" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C13" s="136">
         <v>1</v>
@@ -16670,7 +16670,7 @@
     </row>
     <row r="2" spans="1:15" ht="13" x14ac:dyDescent="0.3">
       <c r="A2" s="40" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
@@ -16763,7 +16763,7 @@
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B5" s="59" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C5" s="136">
         <v>1</v>
@@ -16939,7 +16939,7 @@
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B9" s="90" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C9" s="136">
         <v>1</v>
@@ -17203,7 +17203,7 @@
     </row>
     <row r="16" spans="1:15" ht="13" x14ac:dyDescent="0.3">
       <c r="A16" s="40" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B16" s="59"/>
     </row>
@@ -17442,7 +17442,7 @@
     </row>
     <row r="2" spans="1:7" ht="13" x14ac:dyDescent="0.3">
       <c r="A2" s="40" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -17467,7 +17467,7 @@
     </row>
     <row r="4" spans="1:7" ht="13" x14ac:dyDescent="0.3">
       <c r="A4" s="40" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B4" s="59"/>
       <c r="C4" s="127"/>
@@ -17532,10 +17532,10 @@
         <v>69</v>
       </c>
       <c r="B1" s="40" t="s">
+        <v>264</v>
+      </c>
+      <c r="C1" s="125" t="s">
         <v>265</v>
-      </c>
-      <c r="C1" s="125" t="s">
-        <v>266</v>
       </c>
       <c r="D1" s="40" t="s">
         <v>1</v>
@@ -17561,7 +17561,7 @@
         <v>71</v>
       </c>
       <c r="C2" s="52" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D2" s="136">
         <v>0</v>
@@ -17581,7 +17581,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C3" s="52" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D3" s="136">
         <v>0</v>
@@ -17601,7 +17601,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C4" s="52" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D4" s="136">
         <v>0</v>
@@ -17627,7 +17627,7 @@
         <v>66</v>
       </c>
       <c r="C5" s="52" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D5" s="136">
         <v>0</v>
@@ -17647,7 +17647,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C6" s="52" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D6" s="136">
         <v>0</v>
@@ -17670,7 +17670,7 @@
         <v>65</v>
       </c>
       <c r="C7" s="52" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D7" s="136">
         <v>0</v>
@@ -17690,7 +17690,7 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C8" s="52" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D8" s="136">
         <v>0</v>
@@ -17716,7 +17716,7 @@
         <v>66</v>
       </c>
       <c r="C9" s="52" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D9" s="136">
         <v>0</v>
@@ -17736,7 +17736,7 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C10" s="52" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D10" s="136">
         <v>0</v>
@@ -17759,7 +17759,7 @@
         <v>65</v>
       </c>
       <c r="C11" s="52" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D11" s="136">
         <v>0</v>
@@ -17779,7 +17779,7 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C12" s="52" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D12" s="136">
         <v>0</v>
@@ -17805,7 +17805,7 @@
         <v>66</v>
       </c>
       <c r="C13" s="52" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D13" s="136">
         <v>0</v>
@@ -17825,7 +17825,7 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C14" s="52" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D14" s="136">
         <v>0</v>
@@ -17849,7 +17849,7 @@
         <v>65</v>
       </c>
       <c r="C15" s="52" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D15" s="136">
         <v>0</v>
@@ -17870,7 +17870,7 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C16" s="52" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D16" s="136">
         <v>0</v>
@@ -17897,7 +17897,7 @@
         <v>27</v>
       </c>
       <c r="C17" s="52" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D17" s="136">
         <v>0.7</v>
@@ -17918,7 +17918,7 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C18" s="52" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D18" s="136">
         <v>0.186</v>
@@ -17945,7 +17945,7 @@
         <v>27</v>
       </c>
       <c r="C19" s="52" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D19" s="136">
         <v>0.7</v>
@@ -17965,7 +17965,7 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C20" s="52" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D20" s="136">
         <v>0.186</v>
@@ -17991,7 +17991,7 @@
         <v>27</v>
       </c>
       <c r="C21" s="52" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D21" s="136">
         <v>0.7</v>
@@ -18011,7 +18011,7 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C22" s="52" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D22" s="136">
         <v>0.186</v>
@@ -18037,7 +18037,7 @@
         <v>71</v>
       </c>
       <c r="C23" s="52" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D23" s="136">
         <v>1</v>
@@ -18057,7 +18057,7 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C24" s="52" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D24" s="136">
         <v>0</v>
@@ -18077,7 +18077,7 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C25" s="52" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D25" s="136">
         <v>0</v>
@@ -18103,7 +18103,7 @@
         <v>71</v>
       </c>
       <c r="C26" s="52" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D26" s="136">
         <v>1</v>
@@ -18123,7 +18123,7 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C27" s="52" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D27" s="136">
         <v>0</v>
@@ -18143,7 +18143,7 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C28" s="52" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D28" s="136">
         <v>0</v>
@@ -18169,7 +18169,7 @@
         <v>71</v>
       </c>
       <c r="C29" s="52" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D29" s="136">
         <v>1</v>
@@ -18189,7 +18189,7 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C30" s="52" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D30" s="136">
         <v>0</v>
@@ -18209,7 +18209,7 @@
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C31" s="52" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D31" s="136">
         <v>0</v>
@@ -18235,7 +18235,7 @@
         <v>71</v>
       </c>
       <c r="C32" s="52" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D32" s="136">
         <v>1</v>
@@ -18255,7 +18255,7 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C33" s="52" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D33" s="136">
         <v>0</v>
@@ -18275,7 +18275,7 @@
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C34" s="52" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D34" s="136">
         <v>0</v>
@@ -18301,7 +18301,7 @@
         <v>71</v>
       </c>
       <c r="C35" s="52" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D35" s="136">
         <v>1</v>
@@ -18321,7 +18321,7 @@
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C36" s="52" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D36" s="136">
         <v>0</v>
@@ -18341,7 +18341,7 @@
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C37" s="52" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D37" s="136">
         <v>0</v>
@@ -18367,7 +18367,7 @@
         <v>71</v>
       </c>
       <c r="C38" s="52" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D38" s="136">
         <v>0.3</v>
@@ -18387,7 +18387,7 @@
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C39" s="52" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D39" s="136">
         <v>0.6</v>
@@ -18407,7 +18407,7 @@
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C40" s="52" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D40" s="136">
         <v>0.45</v>
@@ -18430,7 +18430,7 @@
         <v>16</v>
       </c>
       <c r="C41" s="52" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D41" s="136">
         <v>0.3</v>
@@ -18450,7 +18450,7 @@
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C42" s="52" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D42" s="136">
         <v>0.5</v>
@@ -18470,7 +18470,7 @@
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C43" s="52" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D43" s="136">
         <v>0.63</v>
@@ -18496,7 +18496,7 @@
         <v>71</v>
       </c>
       <c r="C44" s="52" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D44" s="136">
         <v>0.88</v>
@@ -18516,7 +18516,7 @@
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C45" s="52" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D45" s="136">
         <v>0.8</v>
@@ -18542,7 +18542,7 @@
         <v>71</v>
       </c>
       <c r="C46" s="52" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D46" s="136">
         <v>1</v>
@@ -18562,7 +18562,7 @@
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C47" s="52" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D47" s="136">
         <v>0.76</v>
@@ -18588,7 +18588,7 @@
         <v>13</v>
       </c>
       <c r="C48" s="52" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D48" s="136">
         <v>0.57999999999999996</v>
@@ -18608,7 +18608,7 @@
     </row>
     <row r="49" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C49" s="52" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D49" s="136">
         <v>0.88</v>
@@ -18658,7 +18658,7 @@
         <v>69</v>
       </c>
       <c r="B1" s="119" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C1" s="119"/>
       <c r="D1" s="40" t="s">
@@ -18683,7 +18683,7 @@
         <v>41</v>
       </c>
       <c r="C2" s="43" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D2" s="136">
         <v>1</v>
@@ -18701,7 +18701,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C3" s="35" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D3" s="136">
         <v>0.2</v>
@@ -18725,7 +18725,7 @@
         <v>41</v>
       </c>
       <c r="C4" s="43" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D4" s="136">
         <v>1</v>
@@ -18744,7 +18744,7 @@
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="36"/>
       <c r="C5" s="35" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D5" s="136">
         <v>0.59</v>
@@ -18768,7 +18768,7 @@
         <v>41</v>
       </c>
       <c r="C6" s="43" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D6" s="136">
         <v>1</v>
@@ -18787,7 +18787,7 @@
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="36"/>
       <c r="C7" s="35" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D7" s="136">
         <v>0.59</v>
@@ -18840,10 +18840,10 @@
     </row>
     <row r="2" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>209</v>
+      </c>
+      <c r="B2" s="41" t="s">
         <v>210</v>
-      </c>
-      <c r="B2" s="41" t="s">
-        <v>211</v>
       </c>
       <c r="C2" s="41" t="s">
         <v>1</v>
@@ -18942,7 +18942,7 @@
         <v>31</v>
       </c>
       <c r="B13" s="41" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C13" s="23" t="s">
         <v>2</v>
@@ -19148,7 +19148,7 @@
         <v>32</v>
       </c>
       <c r="B25" s="41" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C25" s="41" t="s">
         <v>32</v>
@@ -20474,8 +20474,8 @@
   </sheetPr>
   <dimension ref="A1:F39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -20500,7 +20500,7 @@
         <v>200</v>
       </c>
       <c r="D1" s="53" t="s">
-        <v>206</v>
+        <v>271</v>
       </c>
       <c r="E1" s="53" t="s">
         <v>205</v>
@@ -20661,7 +20661,7 @@
     </row>
     <row r="11" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="59" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B11" s="81">
         <v>0</v>
@@ -20729,7 +20729,7 @@
     </row>
     <row r="15" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="11" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B15" s="81">
         <v>0</v>
@@ -21140,7 +21140,7 @@
       <c r="F39" s="36"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="jSdherlZJbZ8Sy1L59bo9v5QauB4K+9LWnSRVPNbXJxTAgxgiv9ErxgnISHZ2apMgabDAJDnLmaWIXWQOwB0iA==" saltValue="GDpAVnNFn9RTLmsUAjB9Mw==" spinCount="100000" sheet="1" scenarios="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="11KK+8YPsWPayRfkTglngxmYKXHrDGDfuRB0aZHm6MFFs2ZkzSdhjVK82lgTOCpg8R9z/N0v81GzaOk7EIUi5g==" saltValue="086D79ZNUpTIRk1q+qTm2g==" spinCount="100000" sheet="1" scenarios="1" selectLockedCells="1"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D38">
     <sortCondition ref="A2:A38"/>
   </sortState>

</xml_diff>

<commit_message>
fixes errors in databook sheet headers
</commit_message>
<xml_diff>
--- a/inputs/demo_demo_input.xlsx
+++ b/inputs/demo_demo_input.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Covid-India-UP\Nutrition\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A05E5E5-A960-4822-BC89-72BBCFD24B6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CFFFCA4-778D-49F6-A921-E22DB339200C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="961" firstSheet="3" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1569,10 +1569,10 @@
     <t>Unit Cost</t>
   </si>
   <si>
-    <t>Max coverage increase per annum</t>
+    <t>Max-increase per annum</t>
   </si>
   <si>
-    <t>Max coverage decrease per annum</t>
+    <t>Max-decrease per annum</t>
   </si>
 </sst>
 </file>
@@ -5601,8 +5601,8 @@
   </sheetPr>
   <dimension ref="A1:G39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J23" sqref="J23"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -16632,6 +16632,42 @@
   </sheetData>
   <sheetProtection selectLockedCells="1"/>
   <mergeCells count="45">
+    <mergeCell ref="B19:B21"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="B14:B16"/>
+    <mergeCell ref="B42:B44"/>
+    <mergeCell ref="B45:B47"/>
+    <mergeCell ref="B48:B50"/>
+    <mergeCell ref="B22:B24"/>
+    <mergeCell ref="B25:B27"/>
+    <mergeCell ref="B28:B30"/>
+    <mergeCell ref="B31:B33"/>
+    <mergeCell ref="B36:B38"/>
+    <mergeCell ref="B39:B41"/>
+    <mergeCell ref="B55:B57"/>
+    <mergeCell ref="B58:B60"/>
+    <mergeCell ref="B61:B63"/>
+    <mergeCell ref="B64:B66"/>
+    <mergeCell ref="B67:B69"/>
+    <mergeCell ref="B72:B74"/>
+    <mergeCell ref="B75:B77"/>
+    <mergeCell ref="B78:B80"/>
+    <mergeCell ref="B81:B83"/>
+    <mergeCell ref="B84:B86"/>
+    <mergeCell ref="B108:B110"/>
+    <mergeCell ref="B89:B91"/>
+    <mergeCell ref="B92:B94"/>
+    <mergeCell ref="B95:B97"/>
+    <mergeCell ref="B98:B100"/>
+    <mergeCell ref="B101:B103"/>
+    <mergeCell ref="B111:B113"/>
+    <mergeCell ref="B114:B116"/>
+    <mergeCell ref="B117:B119"/>
+    <mergeCell ref="B120:B122"/>
+    <mergeCell ref="B125:B127"/>
     <mergeCell ref="B145:B147"/>
     <mergeCell ref="B148:B150"/>
     <mergeCell ref="B151:B153"/>
@@ -16641,42 +16677,6 @@
     <mergeCell ref="B134:B136"/>
     <mergeCell ref="B137:B139"/>
     <mergeCell ref="B142:B144"/>
-    <mergeCell ref="B111:B113"/>
-    <mergeCell ref="B114:B116"/>
-    <mergeCell ref="B117:B119"/>
-    <mergeCell ref="B120:B122"/>
-    <mergeCell ref="B125:B127"/>
-    <mergeCell ref="B108:B110"/>
-    <mergeCell ref="B89:B91"/>
-    <mergeCell ref="B92:B94"/>
-    <mergeCell ref="B95:B97"/>
-    <mergeCell ref="B98:B100"/>
-    <mergeCell ref="B101:B103"/>
-    <mergeCell ref="B72:B74"/>
-    <mergeCell ref="B75:B77"/>
-    <mergeCell ref="B78:B80"/>
-    <mergeCell ref="B81:B83"/>
-    <mergeCell ref="B84:B86"/>
-    <mergeCell ref="B55:B57"/>
-    <mergeCell ref="B58:B60"/>
-    <mergeCell ref="B61:B63"/>
-    <mergeCell ref="B64:B66"/>
-    <mergeCell ref="B67:B69"/>
-    <mergeCell ref="B42:B44"/>
-    <mergeCell ref="B45:B47"/>
-    <mergeCell ref="B48:B50"/>
-    <mergeCell ref="B22:B24"/>
-    <mergeCell ref="B25:B27"/>
-    <mergeCell ref="B28:B30"/>
-    <mergeCell ref="B31:B33"/>
-    <mergeCell ref="B36:B38"/>
-    <mergeCell ref="B39:B41"/>
-    <mergeCell ref="B19:B21"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="B5:B7"/>
-    <mergeCell ref="B8:B10"/>
-    <mergeCell ref="B11:B13"/>
-    <mergeCell ref="B14:B16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>

</xml_diff>